<commit_message>
27 12 2018 10:53 AM
</commit_message>
<xml_diff>
--- a/SelDatUnilever_Ver1.00/Management/TrafficManager/Configure.xlsx
+++ b/SelDatUnilever_Ver1.00/Management/TrafficManager/Configure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luat.tran\source\repos\Unilever\SelDatUnilever_Ver1.00\SelDatUnilever_Ver1.00\Management\TrafficManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luat.tran\Source\Repos\SelDatU_Ver1.00\SelDatUnilever_Ver1.00\Management\TrafficManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>Point4</t>
+  </si>
+  <si>
+    <t>READY</t>
   </si>
 </sst>
 </file>
@@ -641,10 +644,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,10 +793,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B7" s="3">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>43</v>
@@ -807,238 +810,258 @@
       <c r="F7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="3">
         <v>200</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="3">
         <v>100</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="3">
         <v>100</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="3">
         <v>100</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="3">
         <v>100</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="3">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="3">
         <v>10</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="3">
         <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3">
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="3">
         <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="3">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>